<commit_message>
Add comments to files.
</commit_message>
<xml_diff>
--- a/06_source/ADAS/code_documentation/work_split.xlsx
+++ b/06_source/ADAS/code_documentation/work_split.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh SD/Github/ADAS/06_source/ADAS/code_documentation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3656D9A9-6730-D142-B8ED-5BC8A8D37D5B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{BF8A3BAA-18ED-1F40-985D-899202E3FF28}"/>
+    <workbookView xWindow="2775" yWindow="1560" windowWidth="28035" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,7 +194,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -284,13 +278,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -594,34 +588,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916CAE76-F9A4-4147-B5A7-DDB473DBE587}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="7"/>
       <c r="G1" s="5">
         <v>43494</v>
       </c>
@@ -645,7 +639,7 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -811,7 +805,7 @@
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -819,7 +813,7 @@
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -840,7 +834,7 @@
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C28" t="s">
@@ -859,7 +853,7 @@
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -867,7 +861,7 @@
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -875,7 +869,7 @@
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -883,7 +877,7 @@
       <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -939,7 +933,7 @@
       <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -947,7 +941,7 @@
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -971,7 +965,7 @@
       <c r="A44" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -979,7 +973,7 @@
       <c r="A45" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -987,7 +981,7 @@
       <c r="A46" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -995,7 +989,7 @@
       <c r="A47" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="6" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>